<commit_message>
Add testng xml file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sankalpgrover/Projects/restassured-apiautomation/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4F492E-37B1-8E4C-862D-A77090C8DC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F04CB37-34CA-8A48-AA84-193E44F1B3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,9 +29,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
-    <t>Data</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -44,9 +41,6 @@
     <t>status</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>Inactive</t>
   </si>
   <si>
@@ -62,22 +56,28 @@
     <t>Id</t>
   </si>
   <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>Brahmabrata Chaturvedi</t>
-  </si>
-  <si>
-    <t>brahmabrata_chaturvedi@schultz.biz</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
     <t>female</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>khanna_deepankar@senger.co</t>
+  </si>
+  <si>
+    <t>DummyField</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Deepankar Khanna</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -471,38 +471,38 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>11</v>
@@ -510,31 +510,31 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="2"/>

</xml_diff>